<commit_message>
livelihoods and economies update
</commit_message>
<xml_diff>
--- a/Livelihoods/Employment_Figures/Canada/NWT_Employment_2001_2015.xlsx
+++ b/Livelihoods/Employment_Figures/Canada/NWT_Employment_2001_2015.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,6 +208,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -243,6 +260,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,6 +436,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>